<commit_message>
neg flo_cost for UC dummies
</commit_message>
<xml_diff>
--- a/suppxls/Scen_demo_UCs.xlsx
+++ b/suppxls/Scen_demo_UCs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VEDA\Veda\Veda_models\Demo_Adv_Veda\suppxls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC843B79-54F5-4661-AE4C-74DF7584C005}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42C83460-E529-43E0-AA9A-38035093F7DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3900" yWindow="3900" windowWidth="21600" windowHeight="12735" activeTab="1" xr2:uid="{839C8D2E-9453-4DE3-9534-B724417FAD70}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="52">
   <si>
     <t>~UC_Sets: R_E: AllRegions</t>
   </si>
@@ -158,6 +158,30 @@
   </si>
   <si>
     <t>at least 95% of all bio production should be consumed by ELE and CHP plants</t>
+  </si>
+  <si>
+    <t>~TFM_INS</t>
+  </si>
+  <si>
+    <t>attribute</t>
+  </si>
+  <si>
+    <t>pset_pn</t>
+  </si>
+  <si>
+    <t>cset_cn</t>
+  </si>
+  <si>
+    <t>value</t>
+  </si>
+  <si>
+    <t>flo_cost</t>
+  </si>
+  <si>
+    <t>IMPNRGZ</t>
+  </si>
+  <si>
+    <t>UC_all_bio*</t>
   </si>
 </sst>
 </file>
@@ -824,17 +848,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16DA9339-7A14-4564-A40D-78F90CE3BB51}">
-  <dimension ref="C3:K8"/>
+  <dimension ref="C3:K15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="24.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="7.7109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10" bestFit="1" customWidth="1"/>
@@ -917,6 +942,39 @@
         <v>5</v>
       </c>
     </row>
+    <row r="13" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C13" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="14" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C14" t="s">
+        <v>45</v>
+      </c>
+      <c r="D14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E14" t="s">
+        <v>47</v>
+      </c>
+      <c r="F14" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="15" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C15" t="s">
+        <v>49</v>
+      </c>
+      <c r="D15" t="s">
+        <v>50</v>
+      </c>
+      <c r="E15" t="s">
+        <v>51</v>
+      </c>
+      <c r="F15">
+        <v>-100</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>